<commit_message>
Updates: lw and sw attempted fixes
</commit_message>
<xml_diff>
--- a/XML_SpreadSheets/control_signals_template.xlsx
+++ b/XML_SpreadSheets/control_signals_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MIPS_PROCESSOR\XML_SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245402C9-13FF-49F6-BCB5-C026FC13552D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E889D533-963B-49A7-BC50-1BE958973CB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
   <si>
     <t>Instruction</t>
   </si>
@@ -392,6 +392,9 @@
   <si>
     <t>srav, sra</t>
   </si>
+  <si>
+    <t>0x101011</t>
+  </si>
 </sst>
 </file>
 
@@ -461,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -503,6 +506,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,10 +737,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1035,8 +1041,8 @@
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
+      <c r="B6" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Update 10/29/20: Fixed sw, lw, only have sltu and sltiu to fix
</commit_message>
<xml_diff>
--- a/XML_SpreadSheets/control_signals_template.xlsx
+++ b/XML_SpreadSheets/control_signals_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MIPS_PROCESSOR\XML_SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E889D533-963B-49A7-BC50-1BE958973CB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9BBBD8-FB09-44F8-8FBF-75CA4F26E818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
   <si>
     <t>Instruction</t>
   </si>
@@ -392,9 +392,6 @@
   <si>
     <t>srav, sra</t>
   </si>
-  <si>
-    <t>0x101011</t>
-  </si>
 </sst>
 </file>
 
@@ -464,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -508,6 +505,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,10 +737,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1042,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>25</v>
@@ -1987,8 +1987,8 @@
       <c r="D23" s="4">
         <v>1</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>72</v>
+      <c r="E23" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Started on the phase 2 control mips
</commit_message>
<xml_diff>
--- a/XML_SpreadSheets/control_signals_template.xlsx
+++ b/XML_SpreadSheets/control_signals_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MIPS_PROCESSOR\XML_SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9BBBD8-FB09-44F8-8FBF-75CA4F26E818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4535F08-D5C5-43BD-86D0-A9EA6D8C1195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
   <si>
     <t>Instruction</t>
   </si>
@@ -372,25 +372,31 @@
     <t>1101</t>
   </si>
   <si>
-    <t>Requires shifting</t>
-  </si>
-  <si>
-    <t>srl, srav, sll, sra, sllv, srlv, lui</t>
-  </si>
-  <si>
     <t>*lui is a special case: shamt = 16 bits</t>
   </si>
   <si>
-    <t>Left Shift?</t>
+    <t>beq</t>
   </si>
   <si>
-    <t>sll, sllv, lui</t>
+    <t>OPCODE</t>
   </si>
   <si>
-    <t>Signed shifted commands:</t>
+    <t>shamt</t>
   </si>
   <si>
-    <t>srav, sra</t>
+    <t>bne</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>SHAMT</t>
+  </si>
+  <si>
+    <t>jal</t>
+  </si>
+  <si>
+    <t>jr</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -508,6 +514,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,10 +746,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2312,13 +2321,13 @@
     </row>
     <row r="30" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
@@ -2349,12 +2358,14 @@
     </row>
     <row r="31" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="15"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -2387,9 +2398,11 @@
         <v>90</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="15"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -2418,9 +2431,15 @@
       <c r="AC32" s="12"/>
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2449,9 +2468,15 @@
       <c r="AC33" s="3"/>
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>

</xml_diff>

<commit_message>
11/3/2020 - 4:35PM - Changing Sign Extender didn't work, error is still in shift for N_queens.s
</commit_message>
<xml_diff>
--- a/XML_SpreadSheets/control_signals_template.xlsx
+++ b/XML_SpreadSheets/control_signals_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MIPS_PROCESSOR\XML_SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD6447-FFB6-416F-881F-BC556E7CB162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D94488F-E18B-4CA5-9DE5-F08277BB2350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>Instruction</t>
   </si>
@@ -759,10 +759,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2473,8 +2473,8 @@
       <c r="J32" s="17">
         <v>1</v>
       </c>
-      <c r="K32" s="17" t="s">
-        <v>91</v>
+      <c r="K32" s="17">
+        <v>0</v>
       </c>
       <c r="L32" s="17">
         <v>0</v>
@@ -2528,8 +2528,8 @@
       <c r="J33" s="17">
         <v>1</v>
       </c>
-      <c r="K33" s="17" t="s">
-        <v>91</v>
+      <c r="K33" s="17">
+        <v>0</v>
       </c>
       <c r="L33" s="17">
         <v>0</v>
@@ -2583,7 +2583,9 @@
       <c r="J34" s="17">
         <v>1</v>
       </c>
-      <c r="K34" s="17"/>
+      <c r="K34" s="17">
+        <v>0</v>
+      </c>
       <c r="L34" s="17"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>

</xml_diff>

<commit_message>
Updated Processor - jal still not working
</commit_message>
<xml_diff>
--- a/XML_SpreadSheets/control_signals_template.xlsx
+++ b/XML_SpreadSheets/control_signals_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MIPS_PROCESSOR\XML_SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D94488F-E18B-4CA5-9DE5-F08277BB2350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEA0C87-D7A6-452E-A854-47C492565516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,10 +759,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="17" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Updated docs to what they are supposed to be
</commit_message>
<xml_diff>
--- a/XML_SpreadSheets/control_signals_template.xlsx
+++ b/XML_SpreadSheets/control_signals_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MIPS_PROCESSOR\XML_SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEA0C87-D7A6-452E-A854-47C492565516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8367CF53-0DF9-4DBC-8F88-8A7D310E7158}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,13 +396,13 @@
     <t>xx</t>
   </si>
   <si>
-    <t>bne[up]</t>
+    <t>jal</t>
   </si>
   <si>
-    <t>jal[up]</t>
+    <t>jr</t>
   </si>
   <si>
-    <t>jr[up]</t>
+    <t>bne</t>
   </si>
 </sst>
 </file>
@@ -759,10 +759,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="31" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>88</v>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>77</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>14</v>
@@ -2586,7 +2586,9 @@
       <c r="K34" s="17">
         <v>0</v>
       </c>
-      <c r="L34" s="17"/>
+      <c r="L34" s="17">
+        <v>0</v>
+      </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>

</xml_diff>